<commit_message>
Starting with power point and task 1 for 2021 complete
</commit_message>
<xml_diff>
--- a/Data-Visualization-Observation-Task/Data and Information Specialist Data Task.xlsx
+++ b/Data-Visualization-Observation-Task/Data and Information Specialist Data Task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sirja\Documents\Southbridge-Public-Schools-Tasks\Data-Visualization-Observation-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3866AB-61E2-454F-AAC2-E4C9F2B1C364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F84BD24-D7FB-4787-8CFF-6894BCBF6847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Visualization Task" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>2021</cx:v>
+          <cx:v>Beginning Composite Score for 2021</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -279,7 +279,7 @@
               <a:latin typeface="Arial"/>
               <a:cs typeface="Arial"/>
             </a:rPr>
-            <a:t>2021</a:t>
+            <a:t>Beginning Composite Score for 2021</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -325,17 +325,72 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0"/>
-        <cx:title/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Beginning Composite Score Range</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>Beginning Composite Score Range</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
-        <cx:title/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Number of Students</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>Number of Students</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
   </cx:chart>
   <cx:spPr>
     <a:ln w="12700">
@@ -357,7 +412,35 @@
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>End Composite Score for 2021</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>End Composite Score for 2021</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="clusteredColumn" uniqueId="{9663E4D1-E9DB-49F4-A9F7-4BB845EDBABF}">
@@ -367,6 +450,27 @@
               <cx:v>Composite_End</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:dataPt idx="0">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="1">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="2">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
           <cx:dataLabels>
             <cx:visibility seriesName="0" categoryName="0" value="1"/>
           </cx:dataLabels>
@@ -378,17 +482,72 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0"/>
-        <cx:title/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>End Composite Score Range</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>End Composite Score Range</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
-        <cx:title/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Number of Students</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>Number of Students</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -15306,7 +15465,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Task 1 Complete and Starting Task 2
</commit_message>
<xml_diff>
--- a/Data-Visualization-Observation-Task/Data and Information Specialist Data Task.xlsx
+++ b/Data-Visualization-Observation-Task/Data and Information Specialist Data Task.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sirja\Documents\Southbridge-Public-Schools-Tasks\Data-Visualization-Observation-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F84BD24-D7FB-4787-8CFF-6894BCBF6847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74EAE1D-B69E-46FD-AC29-1DEF445B9188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Visualization Task" sheetId="1" r:id="rId1"/>
-    <sheet name="2021" sheetId="2" r:id="rId2"/>
-    <sheet name="2022" sheetId="3" r:id="rId3"/>
+    <sheet name="Composite Score of 2021" sheetId="2" r:id="rId2"/>
+    <sheet name="Composite Score of 2022" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Visualization Task'!$A$1:$N$305</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'2021'!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'2021'!$A$2:$A$136</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'2021'!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'2021'!$B$2:$B$136</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'2022'!$A$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'2022'!$A$2:$A$1048421</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Composite Score of 2021'!$B$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Composite Score of 2021'!$B$2:$B$136</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Composite Score of 2021'!$A$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Composite Score of 2021'!$A$2:$A$136</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Composite Score of 2022'!$A$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Composite Score of 2022'!$A$2:$A$150</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Composite Score of 2022'!$B$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Composite Score of 2022'!$B$2:$B$150</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="36">
   <si>
     <t>District_Name</t>
   </si>
@@ -130,15 +132,6 @@
     <t>Core^ Support</t>
   </si>
   <si>
-    <t xml:space="preserve">40th </t>
-  </si>
-  <si>
-    <t>20th</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> m,mmmmmmmmmm</t>
-  </si>
-  <si>
     <t>Beginning 20th percentile</t>
   </si>
   <si>
@@ -167,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -186,8 +179,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +196,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -213,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -227,6 +232,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -250,7 +257,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -289,7 +296,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{0978DCB4-FAEE-4A8E-A4FE-1FF4E8474B72}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Composite_Beginning</cx:v>
             </cx:txData>
           </cx:tx>
@@ -391,6 +398,7 @@
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
   </cx:chart>
   <cx:spPr>
     <a:ln w="12700">
@@ -407,7 +415,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -446,7 +454,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{9663E4D1-E9DB-49F4-A9F7-4BB845EDBABF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Composite_End</cx:v>
             </cx:txData>
           </cx:tx>
@@ -562,15 +570,58 @@
     </cx:data>
   </cx:chartData>
   <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Beginning Composite Score for 2022</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Beginning Composite Score for 2022</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{3669C8BB-7712-4D26-8F0A-2394A559E4F1}">
+        <cx:series layoutId="clusteredColumn" uniqueId="{7839B8C6-0AC0-4D9F-BD1F-B7ECFE0DA7F7}">
           <cx:tx>
             <cx:txData>
               <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Composite_Beginning</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:dataPt idx="0">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="1">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
           <cx:dataLabels>
             <cx:visibility seriesName="0" categoryName="0" value="1"/>
           </cx:dataLabels>
@@ -582,17 +633,222 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0"/>
-        <cx:title/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Beginning Composite Score Range</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>Beginning Composite Score Range</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
-        <cx:title/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Number of Students </cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>Number of Students </a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>End Composite Score for 2022</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>End Composite Score for 2022</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{804FF728-FA49-4730-A194-E81F18E1B49D}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:v>Composite_End</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataPt idx="0">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="1">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="2">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>End Composite Score Range</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>End Composite Score Range</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Number of Students</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>Number of Students</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -678,6 +934,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2241,20 +2537,528 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2543175</xdr:colOff>
+      <xdr:colOff>2552700</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -2290,7 +3094,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3228976" y="577850"/>
+              <a:off x="3371851" y="549275"/>
               <a:ext cx="5286374" cy="4746625"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2329,8 +3133,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -2368,8 +3172,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9020174" y="581025"/>
-              <a:ext cx="5095875" cy="4724400"/>
+              <a:off x="9153524" y="581025"/>
+              <a:ext cx="5534026" cy="4724400"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2406,25 +3210,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1368425</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>288925</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Chart 1">
+            <xdr:cNvPr id="3" name="Chart 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0974E42E-8920-4760-9432-9BCB7BB83382}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1745AF23-6658-194E-7C5D-204466C0B132}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2451,8 +3255,86 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6578600" y="1701800"/>
-              <a:ext cx="4483100" cy="2838450"/>
+              <a:off x="3371850" y="771525"/>
+              <a:ext cx="5524500" cy="4552950"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{155B4D2B-8C1B-F517-50A7-A92D9AFD7E5A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9410700" y="771525"/>
+              <a:ext cx="6343650" cy="4533899"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2688,14 +3570,21 @@
   </sheetPr>
   <dimension ref="A1:P305"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M1:M1048576"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H316" sqref="H316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="28.140625" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="13" width="25.42578125" customWidth="1"/>
     <col min="14" max="14" width="34.7109375" customWidth="1"/>
     <col min="15" max="15" width="17.140625" customWidth="1"/>
@@ -2744,12 +3633,8 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3030,7 +3915,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -3074,7 +3959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -3162,7 +4047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -3206,7 +4091,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3250,7 +4135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -3291,7 +4176,7 @@
         <v>364</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3334,7 +4219,7 @@
       <c r="M15" s="2">
         <v>369</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="N15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3382,7 +4267,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3426,7 +4311,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -3514,7 +4399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -3602,7 +4487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -4086,7 +4971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -4130,7 +5015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -4294,7 +5179,7 @@
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
     </row>
-    <row r="38" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -4754,7 +5639,7 @@
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
     </row>
-    <row r="49" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>14</v>
       </c>
@@ -4842,7 +5727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>14</v>
       </c>
@@ -4930,7 +5815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>14</v>
       </c>
@@ -5062,7 +5947,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>14</v>
       </c>
@@ -5150,7 +6035,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>14</v>
       </c>
@@ -5194,7 +6079,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>14</v>
       </c>
@@ -5282,7 +6167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>14</v>
       </c>
@@ -5414,7 +6299,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>14</v>
       </c>
@@ -5678,7 +6563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>14</v>
       </c>
@@ -5722,7 +6607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>14</v>
       </c>
@@ -5766,7 +6651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>14</v>
       </c>
@@ -5810,7 +6695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>14</v>
       </c>
@@ -5854,7 +6739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>14</v>
       </c>
@@ -5898,7 +6783,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>14</v>
       </c>
@@ -6030,7 +6915,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>14</v>
       </c>
@@ -6294,7 +7179,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>14</v>
       </c>
@@ -6470,7 +7355,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>14</v>
       </c>
@@ -6602,7 +7487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>14</v>
       </c>
@@ -6646,7 +7531,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>14</v>
       </c>
@@ -6690,7 +7575,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
@@ -6822,7 +7707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>14</v>
       </c>
@@ -6910,7 +7795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>14</v>
       </c>
@@ -7042,7 +7927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>14</v>
       </c>
@@ -7130,7 +8015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>14</v>
       </c>
@@ -7350,7 +8235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>14</v>
       </c>
@@ -7394,7 +8279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>14</v>
       </c>
@@ -7828,7 +8713,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>14</v>
       </c>
@@ -7916,7 +8801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>14</v>
       </c>
@@ -7960,7 +8845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>14</v>
       </c>
@@ -8048,7 +8933,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>14</v>
       </c>
@@ -8092,7 +8977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>14</v>
       </c>
@@ -8224,7 +9109,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>14</v>
       </c>
@@ -8268,7 +9153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>14</v>
       </c>
@@ -8312,7 +9197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>14</v>
       </c>
@@ -8476,7 +9361,7 @@
       <c r="M133" s="4"/>
       <c r="N133" s="4"/>
     </row>
-    <row r="134" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>14</v>
       </c>
@@ -8590,7 +9475,7 @@
       <c r="M136" s="4"/>
       <c r="N136" s="4"/>
     </row>
-    <row r="137" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>14</v>
       </c>
@@ -8634,7 +9519,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>14</v>
       </c>
@@ -8810,7 +9695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>14</v>
       </c>
@@ -8854,7 +9739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>14</v>
       </c>
@@ -9018,7 +9903,7 @@
       <c r="M146" s="4"/>
       <c r="N146" s="4"/>
     </row>
-    <row r="147" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>14</v>
       </c>
@@ -9314,7 +10199,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>14</v>
       </c>
@@ -9402,7 +10287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>14</v>
       </c>
@@ -9490,7 +10375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>14</v>
       </c>
@@ -9534,7 +10419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>14</v>
       </c>
@@ -9578,7 +10463,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>14</v>
       </c>
@@ -9622,7 +10507,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>14</v>
       </c>
@@ -9830,7 +10715,7 @@
       <c r="M165" s="4"/>
       <c r="N165" s="4"/>
     </row>
-    <row r="166" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>14</v>
       </c>
@@ -9874,7 +10759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>14</v>
       </c>
@@ -9962,7 +10847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>14</v>
       </c>
@@ -10006,7 +10891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>14</v>
       </c>
@@ -10050,7 +10935,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>14</v>
       </c>
@@ -10138,7 +11023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>14</v>
       </c>
@@ -10226,7 +11111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>14</v>
       </c>
@@ -10314,7 +11199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>14</v>
       </c>
@@ -10358,7 +11243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>14</v>
       </c>
@@ -10402,7 +11287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>14</v>
       </c>
@@ -10490,7 +11375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>14</v>
       </c>
@@ -10534,7 +11419,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>14</v>
       </c>
@@ -10666,7 +11551,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>14</v>
       </c>
@@ -10754,7 +11639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>14</v>
       </c>
@@ -10798,7 +11683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>14</v>
       </c>
@@ -11018,7 +11903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>14</v>
       </c>
@@ -11194,7 +12079,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>14</v>
       </c>
@@ -11414,7 +12299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>14</v>
       </c>
@@ -11458,7 +12343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>14</v>
       </c>
@@ -11502,7 +12387,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>14</v>
       </c>
@@ -11672,7 +12557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>14</v>
       </c>
@@ -11716,7 +12601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>14</v>
       </c>
@@ -11760,7 +12645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>14</v>
       </c>
@@ -12088,7 +12973,7 @@
       <c r="M217" s="4"/>
       <c r="N217" s="4"/>
     </row>
-    <row r="218" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>14</v>
       </c>
@@ -12220,7 +13105,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>14</v>
       </c>
@@ -12308,7 +13193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>14</v>
       </c>
@@ -12352,7 +13237,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>14</v>
       </c>
@@ -12396,7 +13281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>14</v>
       </c>
@@ -12440,7 +13325,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>14</v>
       </c>
@@ -12528,7 +13413,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>14</v>
       </c>
@@ -12572,7 +13457,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>14</v>
       </c>
@@ -12660,7 +13545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>14</v>
       </c>
@@ -12704,7 +13589,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>14</v>
       </c>
@@ -12748,7 +13633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>14</v>
       </c>
@@ -12968,7 +13853,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>14</v>
       </c>
@@ -13012,7 +13897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>14</v>
       </c>
@@ -13056,7 +13941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>14</v>
       </c>
@@ -13100,7 +13985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>14</v>
       </c>
@@ -13232,7 +14117,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>14</v>
       </c>
@@ -13276,7 +14161,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>14</v>
       </c>
@@ -13496,7 +14381,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>14</v>
       </c>
@@ -13572,7 +14457,7 @@
       <c r="M251" s="4"/>
       <c r="N251" s="4"/>
     </row>
-    <row r="252" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>14</v>
       </c>
@@ -13698,7 +14583,7 @@
       <c r="M254" s="4"/>
       <c r="N254" s="4"/>
     </row>
-    <row r="255" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>14</v>
       </c>
@@ -13742,7 +14627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>14</v>
       </c>
@@ -13950,7 +14835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>14</v>
       </c>
@@ -14038,7 +14923,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>14</v>
       </c>
@@ -14082,7 +14967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>14</v>
       </c>
@@ -14126,7 +15011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>14</v>
       </c>
@@ -14202,7 +15087,7 @@
       <c r="M266" s="4"/>
       <c r="N266" s="4"/>
     </row>
-    <row r="267" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>14</v>
       </c>
@@ -14422,7 +15307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>14</v>
       </c>
@@ -14524,7 +15409,7 @@
       <c r="M274" s="4"/>
       <c r="N274" s="4"/>
     </row>
-    <row r="275" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>14</v>
       </c>
@@ -14906,7 +15791,7 @@
       <c r="M285" s="4"/>
       <c r="N285" s="4"/>
     </row>
-    <row r="286" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>14</v>
       </c>
@@ -14964,7 +15849,7 @@
       <c r="M287" s="4"/>
       <c r="N287" s="4"/>
     </row>
-    <row r="288" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>14</v>
       </c>
@@ -15320,7 +16205,7 @@
       <c r="M300" s="4"/>
       <c r="N300" s="4"/>
     </row>
-    <row r="301" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>14</v>
       </c>
@@ -15378,7 +16263,7 @@
       <c r="M302" s="4"/>
       <c r="N302" s="4"/>
     </row>
-    <row r="303" spans="1:14" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>14</v>
       </c>
@@ -15444,17 +16329,24 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N305" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="2022"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="12">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
   </autoFilter>
+  <conditionalFormatting sqref="B2:P305">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15463,40 +16355,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D102199-9C42-4C75-A29B-D24B6B0F9E8D}">
   <dimension ref="A1:H136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomLeft" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" style="6" customWidth="1"/>
     <col min="5" max="5" width="38.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="7" style="5" customWidth="1"/>
     <col min="7" max="7" width="33.28515625" style="6" customWidth="1"/>
     <col min="8" max="8" width="28.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -16523,1219 +17416,1566 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C583425-45EF-41F4-BC7B-83500CC3053F}">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="45.42578125" customWidth="1"/>
+    <col min="8" max="8" width="50.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>268</v>
       </c>
       <c r="B2" s="2">
         <v>358</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2"/>
+      <c r="D2">
         <f>_xlfn.PERCENTILE.INC(A2:A141, 0.2)</f>
         <v>291.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>_xlfn.PERCENTILE.INC(A2:A141, 0.4)</f>
+        <v>309.2</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2">
+        <f>_xlfn.PERCENTILE.INC(B2:B150, 0.2)</f>
+        <v>395</v>
+      </c>
+      <c r="H2">
+        <f>_xlfn.PERCENTILE.INC(B2:B150, 0.4)</f>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>268</v>
       </c>
       <c r="B3" s="2">
         <v>362</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>273</v>
       </c>
       <c r="B4" s="2">
         <v>413</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>277</v>
       </c>
       <c r="B5" s="2">
         <v>369</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>278</v>
       </c>
       <c r="B6" s="2">
         <v>387</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>279</v>
       </c>
       <c r="B7" s="2">
         <v>370</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>280</v>
       </c>
       <c r="B8" s="2">
         <v>373</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>281</v>
       </c>
       <c r="B9" s="2">
         <v>370</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>281</v>
       </c>
       <c r="B10" s="2">
         <v>372</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>281</v>
       </c>
       <c r="B11" s="2">
         <v>371</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>281</v>
       </c>
       <c r="B12" s="2">
         <v>401</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>282</v>
       </c>
       <c r="B13" s="2">
         <v>371</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>283</v>
       </c>
       <c r="B14" s="2">
         <v>384</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C14" s="2"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>283</v>
       </c>
       <c r="B15" s="2">
         <v>384</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>283</v>
       </c>
       <c r="B16" s="2">
         <v>378</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>283</v>
       </c>
       <c r="B17" s="2">
         <v>392</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>283</v>
       </c>
       <c r="B18" s="2">
         <v>375</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>284</v>
       </c>
       <c r="B19" s="2">
         <v>395</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>284</v>
       </c>
       <c r="B20" s="2">
         <v>393</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>285</v>
       </c>
       <c r="B21" s="2">
         <v>380</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>286</v>
       </c>
       <c r="B22" s="2">
         <v>373</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>287</v>
       </c>
       <c r="B23" s="2">
         <v>399</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>287</v>
       </c>
       <c r="B24" s="2">
         <v>377</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>287</v>
       </c>
       <c r="B25" s="2">
         <v>381</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>289</v>
       </c>
       <c r="B26" s="2">
         <v>386</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>289</v>
       </c>
       <c r="B27" s="2">
         <v>398</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>290</v>
       </c>
       <c r="B28" s="2">
         <v>378</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>291</v>
       </c>
       <c r="B29" s="2">
         <v>396</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>292</v>
       </c>
       <c r="B30" s="2">
         <v>405</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>292</v>
       </c>
       <c r="B31" s="2">
         <v>404</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>293</v>
       </c>
       <c r="B32" s="2">
         <v>395</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C32" s="2"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>294</v>
       </c>
       <c r="B33" s="2">
         <v>415</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C33" s="2"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>295</v>
       </c>
       <c r="B34" s="2">
         <v>390</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C34" s="2"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>295</v>
       </c>
       <c r="B35" s="2">
         <v>408</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C35" s="2"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>297</v>
       </c>
       <c r="B36" s="2">
         <v>395</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C36" s="2"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>297</v>
       </c>
       <c r="B37" s="2">
         <v>409</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C37" s="2"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>297</v>
       </c>
       <c r="B38" s="2">
         <v>459</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C38" s="2"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>298</v>
       </c>
       <c r="B39" s="2">
         <v>409</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C39" s="2"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>298</v>
       </c>
       <c r="B40" s="2">
         <v>399</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C40" s="2"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>300</v>
       </c>
       <c r="B41" s="2">
         <v>407</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C41" s="2"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>300</v>
       </c>
       <c r="B42" s="2">
         <v>428</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C42" s="2"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>302</v>
       </c>
       <c r="B43" s="2">
         <v>412</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C43" s="2"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>302</v>
       </c>
       <c r="B44" s="2">
         <v>440</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C44" s="2"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>302</v>
       </c>
       <c r="B45" s="2">
         <v>418</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C45" s="2"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>302</v>
       </c>
       <c r="B46" s="2">
         <v>403</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C46" s="2"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>302</v>
       </c>
       <c r="B47" s="2">
         <v>404</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C47" s="2"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>303</v>
       </c>
       <c r="B48" s="2">
         <v>416</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C48" s="2"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>303</v>
       </c>
       <c r="B49" s="2">
         <v>407</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C49" s="2"/>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>303</v>
       </c>
       <c r="B50" s="2">
         <v>396</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C50" s="2"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>304</v>
       </c>
       <c r="B51" s="2">
         <v>419</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C51" s="2"/>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>304</v>
       </c>
       <c r="B52" s="2">
         <v>385</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C52" s="2"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>305</v>
       </c>
       <c r="B53" s="2">
         <v>419</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C53" s="2"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>305</v>
       </c>
       <c r="B54" s="2">
         <v>414</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C54" s="2"/>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>306</v>
       </c>
       <c r="B55" s="2">
         <v>427</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C55" s="2"/>
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>307</v>
       </c>
       <c r="B56" s="2">
         <v>425</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C56" s="2"/>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>308</v>
       </c>
       <c r="B57" s="2">
         <v>443</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C57" s="2"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>310</v>
       </c>
       <c r="B58" s="2">
         <v>405</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C58" s="2"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>311</v>
       </c>
       <c r="B59" s="2">
         <v>448</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C59" s="2"/>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>311</v>
       </c>
       <c r="B60" s="2">
         <v>408</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C60" s="2"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>313</v>
       </c>
       <c r="B61" s="2">
         <v>417</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C61" s="2"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>314</v>
       </c>
       <c r="B62" s="2">
         <v>426</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C62" s="2"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>315</v>
       </c>
       <c r="B63" s="2">
         <v>428</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C63" s="2"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>316</v>
       </c>
       <c r="B64" s="2">
         <v>451</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C64" s="2"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>316</v>
       </c>
       <c r="B65" s="2">
         <v>442</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C65" s="2"/>
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>316</v>
       </c>
       <c r="B66" s="2">
         <v>433</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C66" s="2"/>
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>317</v>
       </c>
       <c r="B67" s="2">
         <v>417</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C67" s="2"/>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>318</v>
       </c>
       <c r="B68" s="2">
         <v>432</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C68" s="2"/>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>318</v>
       </c>
       <c r="B69" s="2">
         <v>428</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C69" s="2"/>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>318</v>
       </c>
       <c r="B70" s="2">
         <v>454</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C70" s="2"/>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>319</v>
       </c>
       <c r="B71" s="2">
         <v>424</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C71" s="2"/>
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>321</v>
       </c>
       <c r="B72" s="2">
         <v>432</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C72" s="2"/>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>323</v>
       </c>
       <c r="B73" s="2">
         <v>425</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C73" s="2"/>
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>323</v>
       </c>
       <c r="B74" s="2">
         <v>433</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C74" s="2"/>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>325</v>
       </c>
       <c r="B75" s="2">
         <v>411</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C75" s="2"/>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>325</v>
       </c>
       <c r="B76" s="2">
         <v>437</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C76" s="2"/>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>327</v>
       </c>
       <c r="B77" s="2">
         <v>446</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C77" s="2"/>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>327</v>
       </c>
       <c r="B78" s="2">
         <v>425</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C78" s="2"/>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>327</v>
       </c>
       <c r="B79" s="2">
         <v>447</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C79" s="2"/>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>328</v>
       </c>
       <c r="B80" s="2">
         <v>428</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C80" s="2"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>328</v>
       </c>
       <c r="B81" s="2">
         <v>433</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C81" s="2"/>
+      <c r="F81" s="7"/>
+    </row>
+    <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>330</v>
       </c>
       <c r="B82" s="2">
         <v>455</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C82" s="2"/>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>331</v>
       </c>
       <c r="B83" s="2">
         <v>454</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C83" s="2"/>
+      <c r="F83" s="7"/>
+    </row>
+    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>332</v>
       </c>
       <c r="B84" s="2">
         <v>434</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C84" s="2"/>
+      <c r="F84" s="7"/>
+    </row>
+    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>332</v>
       </c>
       <c r="B85" s="2">
         <v>423</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C85" s="2"/>
+      <c r="F85" s="7"/>
+    </row>
+    <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>332</v>
       </c>
       <c r="B86" s="2">
         <v>433</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C86" s="2"/>
+      <c r="F86" s="7"/>
+    </row>
+    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>333</v>
       </c>
       <c r="B87" s="2">
         <v>443</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C87" s="2"/>
+      <c r="F87" s="7"/>
+    </row>
+    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>334</v>
       </c>
       <c r="B88" s="2">
         <v>422</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C88" s="2"/>
+      <c r="F88" s="7"/>
+    </row>
+    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>336</v>
       </c>
       <c r="B89" s="2">
         <v>451</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C89" s="2"/>
+      <c r="F89" s="7"/>
+    </row>
+    <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>337</v>
       </c>
       <c r="B90" s="2">
         <v>439</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C90" s="2"/>
+      <c r="F90" s="7"/>
+    </row>
+    <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>337</v>
       </c>
       <c r="B91" s="2">
         <v>435</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C91" s="2"/>
+      <c r="F91" s="7"/>
+    </row>
+    <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>338</v>
       </c>
       <c r="B92" s="2">
         <v>443</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C92" s="2"/>
+      <c r="F92" s="7"/>
+    </row>
+    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>339</v>
       </c>
       <c r="B93" s="2">
         <v>452</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C93" s="2"/>
+      <c r="F93" s="7"/>
+    </row>
+    <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>340</v>
       </c>
       <c r="B94" s="2">
         <v>443</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C94" s="2"/>
+      <c r="F94" s="7"/>
+    </row>
+    <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>342</v>
       </c>
       <c r="B95" s="2">
         <v>544</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C95" s="2"/>
+      <c r="F95" s="7"/>
+    </row>
+    <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>344</v>
       </c>
       <c r="B96" s="2">
         <v>443</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C96" s="2"/>
+      <c r="F96" s="7"/>
+    </row>
+    <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>346</v>
       </c>
       <c r="B97" s="2">
         <v>455</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C97" s="2"/>
+      <c r="F97" s="7"/>
+    </row>
+    <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>347</v>
       </c>
       <c r="B98" s="2">
         <v>441</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C98" s="2"/>
+      <c r="F98" s="7"/>
+    </row>
+    <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>348</v>
       </c>
       <c r="B99" s="2">
         <v>444</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C99" s="2"/>
+      <c r="F99" s="7"/>
+    </row>
+    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>349</v>
       </c>
       <c r="B100" s="2">
         <v>478</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C100" s="2"/>
+      <c r="F100" s="7"/>
+    </row>
+    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>349</v>
       </c>
       <c r="B101" s="2">
         <v>453</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C101" s="2"/>
+      <c r="F101" s="7"/>
+    </row>
+    <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>349</v>
       </c>
       <c r="B102" s="2">
         <v>453</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C102" s="2"/>
+      <c r="F102" s="7"/>
+    </row>
+    <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>349</v>
       </c>
       <c r="B103" s="2">
         <v>464</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C103" s="2"/>
+      <c r="F103" s="7"/>
+    </row>
+    <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>350</v>
       </c>
       <c r="B104" s="2">
         <v>455</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C104" s="2"/>
+      <c r="F104" s="7"/>
+    </row>
+    <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>350</v>
       </c>
       <c r="B105" s="2">
         <v>440</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C105" s="2"/>
+      <c r="F105" s="7"/>
+    </row>
+    <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>350</v>
       </c>
       <c r="B106" s="2">
         <v>463</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C106" s="2"/>
+      <c r="F106" s="7"/>
+    </row>
+    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>351</v>
       </c>
       <c r="B107" s="2">
         <v>445</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C107" s="2"/>
+      <c r="F107" s="7"/>
+    </row>
+    <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>351</v>
       </c>
       <c r="B108" s="2">
         <v>454</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C108" s="2"/>
+      <c r="F108" s="7"/>
+    </row>
+    <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>351</v>
       </c>
       <c r="B109" s="2">
         <v>463</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C109" s="2"/>
+      <c r="F109" s="7"/>
+    </row>
+    <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>351</v>
       </c>
       <c r="B110" s="2">
         <v>488</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C110" s="2"/>
+      <c r="F110" s="7"/>
+    </row>
+    <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>352</v>
       </c>
       <c r="B111" s="2">
         <v>504</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C111" s="2"/>
+      <c r="F111" s="7"/>
+    </row>
+    <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>352</v>
       </c>
       <c r="B112" s="2">
         <v>447</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C112" s="2"/>
+      <c r="F112" s="7"/>
+    </row>
+    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>353</v>
       </c>
       <c r="B113" s="2">
         <v>484</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C113" s="2"/>
+      <c r="F113" s="7"/>
+    </row>
+    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>353</v>
       </c>
       <c r="B114" s="2">
         <v>450</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C114" s="2"/>
+      <c r="F114" s="7"/>
+    </row>
+    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>356</v>
       </c>
       <c r="B115" s="2">
         <v>462</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C115" s="2"/>
+      <c r="F115" s="7"/>
+    </row>
+    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>356</v>
       </c>
       <c r="B116" s="2">
         <v>463</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C116" s="2"/>
+      <c r="F116" s="7"/>
+    </row>
+    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>357</v>
       </c>
       <c r="B117" s="2">
         <v>449</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C117" s="2"/>
+      <c r="F117" s="7"/>
+    </row>
+    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>358</v>
       </c>
       <c r="B118" s="2">
         <v>434</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C118" s="2"/>
+      <c r="F118" s="7"/>
+    </row>
+    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>358</v>
       </c>
       <c r="B119" s="2">
         <v>449</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C119" s="2"/>
+      <c r="F119" s="7"/>
+    </row>
+    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>359</v>
       </c>
       <c r="B120" s="2">
         <v>488</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C120" s="2"/>
+      <c r="F120" s="7"/>
+    </row>
+    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>361</v>
       </c>
       <c r="B121" s="2">
         <v>461</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C121" s="2"/>
+      <c r="F121" s="7"/>
+    </row>
+    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>364</v>
       </c>
       <c r="B122" s="2">
         <v>470</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C122" s="2"/>
+      <c r="F122" s="7"/>
+    </row>
+    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>367</v>
       </c>
       <c r="B123" s="2">
         <v>460</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C123" s="2"/>
+      <c r="F123" s="7"/>
+    </row>
+    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>367</v>
       </c>
       <c r="B124" s="2">
         <v>468</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C124" s="2"/>
+      <c r="F124" s="7"/>
+    </row>
+    <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>368</v>
       </c>
       <c r="B125" s="2">
         <v>483</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C125" s="2"/>
+      <c r="F125" s="7"/>
+    </row>
+    <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>369</v>
       </c>
       <c r="B126" s="2">
         <v>454</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C126" s="2"/>
+      <c r="F126" s="7"/>
+    </row>
+    <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>372</v>
       </c>
       <c r="B127" s="2">
         <v>477</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C127" s="2"/>
+      <c r="F127" s="7"/>
+    </row>
+    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>372</v>
       </c>
       <c r="B128" s="2">
         <v>509</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C128" s="2"/>
+      <c r="F128" s="7"/>
+    </row>
+    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>375</v>
       </c>
       <c r="B129" s="2">
         <v>485</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C129" s="2"/>
+      <c r="F129" s="7"/>
+    </row>
+    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>376</v>
       </c>
       <c r="B130" s="2">
         <v>496</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C130" s="2"/>
+      <c r="F130" s="7"/>
+    </row>
+    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>376</v>
       </c>
       <c r="B131" s="2">
         <v>544</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C131" s="2"/>
+      <c r="F131" s="7"/>
+    </row>
+    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>376</v>
       </c>
       <c r="B132" s="2">
         <v>480</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C132" s="2"/>
+      <c r="F132" s="7"/>
+    </row>
+    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>379</v>
       </c>
       <c r="B133" s="2">
         <v>492</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C133" s="2"/>
+      <c r="F133" s="7"/>
+    </row>
+    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>384</v>
       </c>
       <c r="B134" s="2">
         <v>486</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C134" s="2"/>
+      <c r="F134" s="7"/>
+    </row>
+    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>385</v>
       </c>
       <c r="B135" s="2">
         <v>511</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C135" s="2"/>
+      <c r="F135" s="7"/>
+    </row>
+    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>386</v>
       </c>
       <c r="B136" s="2">
         <v>510</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C136" s="2"/>
+      <c r="F136" s="7"/>
+    </row>
+    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>387</v>
       </c>
       <c r="B137" s="2">
         <v>485</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C137" s="2"/>
+      <c r="F137" s="7"/>
+    </row>
+    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>400</v>
       </c>
       <c r="B138" s="2">
         <v>519</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C138" s="2"/>
+      <c r="F138" s="7"/>
+    </row>
+    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>412</v>
       </c>
       <c r="B139" s="2">
         <v>501</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C139" s="2"/>
+      <c r="F139" s="7"/>
+    </row>
+    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>427</v>
       </c>
       <c r="B140" s="2">
         <v>525</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C140" s="2"/>
+      <c r="F140" s="7"/>
+    </row>
+    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>448</v>
       </c>
       <c r="B141" s="2">
         <v>558</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C141" s="2"/>
+      <c r="F141" s="7"/>
+    </row>
+    <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" s="2">
         <v>387</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C142" s="2"/>
+      <c r="F142" s="7"/>
+    </row>
+    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
       <c r="B143" s="2">
         <v>369</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C143" s="2"/>
+      <c r="F143" s="7"/>
+    </row>
+    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
       <c r="B144" s="2">
         <v>431</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C144" s="2"/>
+      <c r="F144" s="7"/>
+    </row>
+    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
       <c r="B145" s="2">
         <v>363</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C145" s="2"/>
+      <c r="F145" s="7"/>
+    </row>
+    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="4"/>
       <c r="B146" s="2">
         <v>425</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C146" s="2"/>
+      <c r="F146" s="7"/>
+    </row>
+    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="4"/>
       <c r="B147" s="2">
         <v>412</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C147" s="2"/>
+      <c r="F147" s="7"/>
+    </row>
+    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="4"/>
       <c r="B148" s="2">
         <v>388</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C148" s="2"/>
+      <c r="F148" s="7"/>
+    </row>
+    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="4"/>
       <c r="B149" s="2">
         <v>414</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="C149" s="2"/>
+      <c r="F149" s="7"/>
+    </row>
+    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="4"/>
       <c r="B150" s="2">
         <v>458</v>
       </c>
+      <c r="C150" s="2"/>
+      <c r="F150" s="7"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F151" s="7"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F152" s="7"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F153" s="7"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F154" s="7"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F155" s="7"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F156" s="7"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F157" s="7"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F158" s="7"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F159" s="7"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F160" s="7"/>
+    </row>
+    <row r="161" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F161" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>